<commit_message>
Manejador de errores arreglado, vector de tokens reconoce los tokens compuestos y separacion de datos.
</commit_message>
<xml_diff>
--- a/Transiton Matrix.xlsx
+++ b/Transiton Matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Documents\Proyectos\Language Programing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA817A6C-83B1-4A7A-B4D8-4CBBA5ACA831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81FB253D-E81A-4E16-BFF2-89DEDA298390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="970" yWindow="2730" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -416,8 +416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="53" zoomScaleNormal="53" workbookViewId="0">
-      <selection activeCell="Y1" sqref="A1:Y1"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="53" zoomScaleNormal="53" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -989,7 +989,7 @@
         <v>100</v>
       </c>
       <c r="F9">
-        <v>-200</v>
+        <v>100</v>
       </c>
       <c r="G9">
         <v>-4</v>
@@ -1057,7 +1057,7 @@
         <v>100</v>
       </c>
       <c r="F10">
-        <v>-200</v>
+        <v>100</v>
       </c>
       <c r="G10">
         <v>-4</v>
@@ -1125,7 +1125,7 @@
         <v>500</v>
       </c>
       <c r="F11">
-        <v>-200</v>
+        <v>500</v>
       </c>
       <c r="G11">
         <v>-200</v>
@@ -1193,7 +1193,7 @@
         <v>100</v>
       </c>
       <c r="F12">
-        <v>-200</v>
+        <v>100</v>
       </c>
       <c r="G12">
         <v>-200</v>
@@ -1261,7 +1261,7 @@
         <v>100</v>
       </c>
       <c r="F13">
-        <v>-200</v>
+        <v>100</v>
       </c>
       <c r="G13">
         <v>-200</v>
@@ -1329,7 +1329,7 @@
         <v>100</v>
       </c>
       <c r="F14">
-        <v>-200</v>
+        <v>100</v>
       </c>
       <c r="G14">
         <v>-200</v>
@@ -1397,7 +1397,7 @@
         <v>100</v>
       </c>
       <c r="F15">
-        <v>-200</v>
+        <v>100</v>
       </c>
       <c r="G15">
         <v>-200</v>
@@ -1465,7 +1465,7 @@
         <v>100</v>
       </c>
       <c r="F16">
-        <v>-200</v>
+        <v>100</v>
       </c>
       <c r="G16">
         <v>-200</v>
@@ -1533,7 +1533,7 @@
         <v>100</v>
       </c>
       <c r="F17">
-        <v>-200</v>
+        <v>100</v>
       </c>
       <c r="G17">
         <v>-200</v>

</xml_diff>